<commit_message>
few further plot modifs
</commit_message>
<xml_diff>
--- a/Robotic arm/BOSCH laser measurements/BOSCH measurement plots.xlsx
+++ b/Robotic arm/BOSCH laser measurements/BOSCH measurement plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aneesh\Desktop\HiWi_Repository\Robotic arm\BOSCH laser measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C423F185-0A66-4A2B-A6BF-D8612B43465E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46881E3E-02D2-44D2-88A5-B2FC96BF18A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8.1 Kgs" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -117,7 +117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1066,7 +1066,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1188,7 +1188,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1348,7 +1348,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1648,7 +1648,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1770,7 +1770,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1930,7 +1930,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2230,7 +2230,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2279,6 +2279,7 @@
         <c:axId val="745829583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.30000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2352,7 +2353,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-IN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2396,6 +2397,7 @@
         <c:crossAx val="745829103"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5055,7 +5057,7 @@
   <dimension ref="C3:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>